<commit_message>
Added possibility to add and change family members information, medical documents and army_orders. Also fixed a lot of bugs, maybe not all
</commit_message>
<xml_diff>
--- a/bases/personal_file.xlsx
+++ b/bases/personal_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,24 +589,18 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1111</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>285463</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1111</v>
+      </c>
+      <c r="C4" t="n">
+        <v>285463</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Екатерингбург</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -634,10 +628,8 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>88005553537</t>
-        </is>
+      <c r="J4" t="n">
+        <v>88005553537</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -744,108 +736,212 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>111</v>
-      </c>
-      <c r="C7" t="n">
-        <v>111</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>gfsf</t>
+          <t>ahgdsfhgsd</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>vxcsdf</t>
+          <t>aaaaa</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>vxcsdf</t>
+          <t>ahgdsfhwdfiuhvdngsd</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>dsfcxvsd</t>
+          <t>nfwebcxsow</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>fgsdg</t>
+          <t>uwdhcvbsnkas</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>cxfsdf</t>
+          <t>mcxqucnxjanksjweidjsbancjsdn</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>cxvsdfsdg</t>
+          <t>saduqwbdas</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>cvadsfsdf</t>
+          <t>mcxqucnxjanksjweidjsbancjsdn</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>asfsdf</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>saasas</t>
-        </is>
+        <v>10</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1111</v>
+      </c>
+      <c r="C8" t="n">
+        <v>123123</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>sdgsgcxv</t>
+          <t>gwerewrfsfg</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dsferhf</t>
+          <t>whfdgsdf</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>cvbvsdgcb</t>
+          <t>vcxht4uf</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>sdfcxvsd</t>
+          <t>vcxfasfs</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>gxcvsd</t>
+          <t>sdgdfijcjmvs</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>fgcxvsdfdfs</t>
+          <t>dgduhsdcjsnskdf</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>bsdfsdg</t>
+          <t>vjsidwhefsjs</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>thytjgfhbvr</t>
+          <t>fsudhfsdjnasjsni</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1212</v>
+      </c>
+      <c r="C9" t="n">
+        <v>151234</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>fsdgsdhsj</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sfkghljfkyurj</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>fmndgfyst</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>gdkeyjhdfh</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>jetykgdhgfj</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>jstrbvssgh</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>dtyijdseg</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>gfhnfgjrstt</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2323</v>
+      </c>
+      <c r="C10" t="n">
+        <v>124167</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>gadfgb</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Moscow</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>bxcvbsdfvbx</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>xvcbsdfg</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>bvxdfagb</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>asfhhhagchawbchanwjenfj</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>xdfsgg</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>asfhhhagchawbchanwjenfj</t>
         </is>
       </c>
     </row>

</xml_diff>